<commit_message>
hepsiemlak veri çekme başarılı olundu
</commit_message>
<xml_diff>
--- a/emlak_ozet.xlsx
+++ b/emlak_ozet.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1357,6 +1357,627 @@
         <v>4944900</v>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>adana</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>ceyhan</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>emlakjet</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>10</v>
+      </c>
+      <c r="E41" t="n">
+        <v>5679900</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>adana</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>kozan</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>emlakjet</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>10</v>
+      </c>
+      <c r="E42" t="n">
+        <v>3211000</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>adiyaman</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>kahta</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>emlakjet</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>10</v>
+      </c>
+      <c r="E43" t="n">
+        <v>3640500</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>adana</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>aladağ</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>emlakjet</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>10</v>
+      </c>
+      <c r="E44" t="n">
+        <v>3028000</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>adana</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>feke</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>emlakjet</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>10</v>
+      </c>
+      <c r="E45" t="n">
+        <v>2832500</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>afyonkarahisar</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>ihsaniye</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>emlakjet</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>10</v>
+      </c>
+      <c r="E46" t="n">
+        <v>3965000</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>adana</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>feke</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>emlakjet</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>3</v>
+      </c>
+      <c r="E47" t="n">
+        <v>2050000</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>adana</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>aladağ</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>emlakjet</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>1</v>
+      </c>
+      <c r="E48" t="n">
+        <v>5150000</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>afyonkarahisar</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>iscehisar</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>emlakjet</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>1</v>
+      </c>
+      <c r="E49" t="n">
+        <v>1150000</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>şırnak</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>uludere</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>emlakjet</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>1</v>
+      </c>
+      <c r="E50" t="n">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>adana</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>ceyhan</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>hepsiemlak</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>10</v>
+      </c>
+      <c r="E51" t="n">
+        <v>5335000</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>istanbul</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>kadıköy</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>hepsiemlak</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>10</v>
+      </c>
+      <c r="E52" t="n">
+        <v>20910000</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>adana</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>ceyhan</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>hepsiemlak</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>10</v>
+      </c>
+      <c r="E53" t="n">
+        <v>5335000</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>istanbul</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>üsküdar</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>hepsiemlak</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>10</v>
+      </c>
+      <c r="E54" t="n">
+        <v>13387500</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>adana</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>ceyhan</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>hepsiemlak</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>10</v>
+      </c>
+      <c r="E55" t="n">
+        <v>4214000</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>istanbul</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>kartal</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>hepsiemlak</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>10</v>
+      </c>
+      <c r="E56" t="n">
+        <v>5980000</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>adana</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>kozan</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>hepsiemlak</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>10</v>
+      </c>
+      <c r="E57" t="n">
+        <v>3051500</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>adana</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>ceyhan</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>hepsiemlak</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>10</v>
+      </c>
+      <c r="E58" t="n">
+        <v>5670000</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>istanbul</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>kadıköy</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>hepsiemlak</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>10</v>
+      </c>
+      <c r="E59" t="n">
+        <v>20590000</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>adana</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>ceyhan</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>hepsiemlak</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>10</v>
+      </c>
+      <c r="E60" t="n">
+        <v>5615000</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>adana</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>ceyhan</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>hepsiemlak</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>10</v>
+      </c>
+      <c r="E61" t="n">
+        <v>5555000</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>adana</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>ceyhan</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>hepsiemlak</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>10</v>
+      </c>
+      <c r="E62" t="n">
+        <v>4734000</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>istanbul</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>ümraniye</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>hepsiemlak</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>10</v>
+      </c>
+      <c r="E63" t="n">
+        <v>14121900</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>adana</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>aladağ</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>hepsiemlak</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>10</v>
+      </c>
+      <c r="E64" t="n">
+        <v>7036500</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>adana</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>feke</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>hepsiemlak</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>1</v>
+      </c>
+      <c r="E65" t="n">
+        <v>5500000</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>adana</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>feke</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>hepsiemlak</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>1</v>
+      </c>
+      <c r="E66" t="n">
+        <v>5500000</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>adana</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>ceyhan</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>hepsiemlak</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>10</v>
+      </c>
+      <c r="E67" t="n">
+        <v>4650000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>